<commit_message>
declaracion esfuerzo 2 final
</commit_message>
<xml_diff>
--- a/Docs/Copia de DeclaracionEsfuerzo.xlsx
+++ b/Docs/Copia de DeclaracionEsfuerzo.xlsx
@@ -56,22 +56,22 @@
     <t>Programa de cerradura (Simulado a través de wiring)</t>
   </si>
   <si>
-    <t>Programa de hub (Simulado a través de nodered)</t>
+    <t>Programa de hub Python</t>
   </si>
   <si>
     <t>Servidores de mensajería (Por ejemplo, Mosquitto, Kafka)</t>
   </si>
   <si>
-    <t>Programa P</t>
-  </si>
-  <si>
-    <t>Código de notificación</t>
-  </si>
-  <si>
-    <t>Código de persistencia</t>
-  </si>
-  <si>
-    <t>Documentación</t>
+    <t>Programa cerradura</t>
+  </si>
+  <si>
+    <t>Hearbeats</t>
+  </si>
+  <si>
+    <t>Servicios REST</t>
+  </si>
+  <si>
+    <t>Pruebas postman</t>
   </si>
   <si>
     <t>Montaje físico de cerradura</t>
@@ -141,7 +141,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -192,6 +192,9 @@
     </xf>
     <xf borderId="4" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="4" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
@@ -213,6 +216,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -466,7 +472,7 @@
       <c r="A13" s="14">
         <v>2.0</v>
       </c>
-      <c r="B13" s="15" t="s">
+      <c r="B13" s="17" t="s">
         <v>14</v>
       </c>
       <c r="C13" s="16"/>
@@ -500,7 +506,7 @@
       <c r="A15" s="14">
         <v>4.0</v>
       </c>
-      <c r="B15" s="13" t="s">
+      <c r="B15" s="18" t="s">
         <v>16</v>
       </c>
       <c r="C15" s="11"/>
@@ -517,7 +523,7 @@
       <c r="A16" s="14">
         <v>5.0</v>
       </c>
-      <c r="B16" s="15" t="s">
+      <c r="B16" s="17" t="s">
         <v>17</v>
       </c>
       <c r="C16" s="11"/>
@@ -534,7 +540,7 @@
       <c r="A17" s="14">
         <v>6.0</v>
       </c>
-      <c r="B17" s="15" t="s">
+      <c r="B17" s="17" t="s">
         <v>18</v>
       </c>
       <c r="C17" s="11"/>
@@ -551,7 +557,7 @@
       <c r="A18" s="14">
         <v>7.0</v>
       </c>
-      <c r="B18" s="13" t="s">
+      <c r="B18" s="18" t="s">
         <v>19</v>
       </c>
       <c r="C18" s="11"/>
@@ -568,7 +574,7 @@
       <c r="A19" s="14">
         <v>8.0</v>
       </c>
-      <c r="B19" s="17" t="s">
+      <c r="B19" s="18" t="s">
         <v>20</v>
       </c>
       <c r="C19" s="16"/>
@@ -585,7 +591,7 @@
       <c r="A20" s="14">
         <v>9.0</v>
       </c>
-      <c r="B20" s="18" t="s">
+      <c r="B20" s="19" t="s">
         <v>21</v>
       </c>
       <c r="C20" s="11"/>
@@ -599,7 +605,7 @@
       <c r="K20" s="11"/>
     </row>
     <row r="21">
-      <c r="A21" s="18"/>
+      <c r="A21" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>